<commit_message>
Added logic for take screenshots of Failed Test cases
</commit_message>
<xml_diff>
--- a/src/main/java/TestData/HalfEbayTestData.xlsx
+++ b/src/main/java/TestData/HalfEbayTestData.xlsx
@@ -12,7 +12,6 @@
     <sheet name="HomePage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -112,6 +111,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="12"/>
@@ -151,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -159,17 +161,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,455 +470,455 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11" style="4"/>
+    <col min="7" max="7" width="11" style="6"/>
     <col min="8" max="8" width="15.875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5">
         <v>94085</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5">
         <v>94086</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4">
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5">
         <v>94087</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="5">
         <v>94088</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5">
         <v>94085</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="5">
         <v>94086</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="4">
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="5">
         <v>94087</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="4">
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="5">
         <v>94088</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="4">
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="5">
         <v>94085</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="4">
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="5">
         <v>94086</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="4">
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="5">
         <v>94087</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="4">
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="5">
         <v>94088</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="4">
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="5">
         <v>94085</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="4">
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="5">
         <v>94086</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="4">
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="5">
         <v>94087</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="4">
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="5">
         <v>94088</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>